<commit_message>
Graf životů - Simulace Válečník VS Lučištník
</commit_message>
<xml_diff>
--- a/valecnikVSlucistnik.xlsx
+++ b/valecnikVSlucistnik.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stepa\Desktop\vyzkumak\vyzkumnyukol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FFBEC83-DABF-4D2D-AA6E-DA4E0B09AFE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06EB5F6-66A6-4F75-A14D-46EBFE930C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8F95D2D3-74D3-478A-BF18-0B60186BD922}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId3"/>
+    <pivotCache cacheId="8" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="25">
   <si>
     <t>id_simulace</t>
   </si>
@@ -202,6 +202,1215 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="cs-CZ"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[valecnikVSlucistnik.xlsx]prubeh_simulaci_Válečník_vs_Luč!Kontingenční tabulka3</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="cs-CZ"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="cs-CZ"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>prubeh_simulaci_Válečník_vs_Luč!$R$3:$R$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>lucisnik</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>prubeh_simulaci_Válečník_vs_Luč!$Q$5:$Q$18</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>prubeh_simulaci_Válečník_vs_Luč!$R$5:$R$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DBAB-4159-B700-8D9D65DBAE9C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>prubeh_simulaci_Válečník_vs_Luč!$S$3:$S$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>valecnik</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>prubeh_simulaci_Válečník_vs_Luč!$Q$5:$Q$18</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>prubeh_simulaci_Válečník_vs_Luč!$S$5:$S$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DBAB-4159-B700-8D9D65DBAE9C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1707439647"/>
+        <c:axId val="1707447807"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1707439647"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="cs-CZ"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1707447807"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1707447807"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="cs-CZ"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1707439647"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="cs-CZ"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="cs-CZ"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graf 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84804AA6-825C-146C-DB99-C6846514E749}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="stepa" refreshedDate="45812.937510185184" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="50" xr:uid="{DB6B6BAC-AED5-42C4-89A9-DBC7DB43E4B1}">
   <cacheSource type="worksheet">
@@ -1033,7 +2242,160 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7761A793-5A97-4F4E-9C9B-64912D226D59}" name="Kontingenční tabulka2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Hodnoty" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{04294842-A07C-43EE-AEE9-0DAF4D1557A2}" name="Kontingenční tabulka3" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Hodnoty" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+  <location ref="Q3:T18" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="13">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="14">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="14">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="3"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" item="2" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Součet z celkove_zivoty" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="2">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7761A793-5A97-4F4E-9C9B-64912D226D59}" name="Kontingenční tabulka2" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Hodnoty" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A57:O68" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -1539,10 +2901,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90FD6D2C-5F1C-43AC-8F05-2398861163D0}">
-  <dimension ref="A1:O68"/>
+  <dimension ref="A1:T68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="S57" sqref="S57"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1551,9 +2913,25 @@
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="3" max="14" width="3" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="31" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1593,8 +2971,14 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1635,7 +3019,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1675,8 +3059,14 @@
       <c r="M3" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1716,8 +3106,20 @@
       <c r="M4" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R4" t="s">
+        <v>14</v>
+      </c>
+      <c r="S4" t="s">
+        <v>17</v>
+      </c>
+      <c r="T4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1757,8 +3159,20 @@
       <c r="M5" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q5" s="2">
+        <v>0</v>
+      </c>
+      <c r="R5" s="4">
+        <v>10</v>
+      </c>
+      <c r="S5" s="4">
+        <v>15</v>
+      </c>
+      <c r="T5" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1798,8 +3212,20 @@
       <c r="M6" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q6" s="2">
+        <v>1</v>
+      </c>
+      <c r="R6" s="4">
+        <v>10</v>
+      </c>
+      <c r="S6" s="4">
+        <v>15</v>
+      </c>
+      <c r="T6" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1839,8 +3265,20 @@
       <c r="M7" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q7" s="2">
+        <v>2</v>
+      </c>
+      <c r="R7" s="4">
+        <v>10</v>
+      </c>
+      <c r="S7" s="4">
+        <v>15</v>
+      </c>
+      <c r="T7" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1880,8 +3318,20 @@
       <c r="M8" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q8" s="2">
+        <v>3</v>
+      </c>
+      <c r="R8" s="4">
+        <v>10</v>
+      </c>
+      <c r="S8" s="4">
+        <v>15</v>
+      </c>
+      <c r="T8" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1921,8 +3371,20 @@
       <c r="M9" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q9" s="2">
+        <v>4</v>
+      </c>
+      <c r="R9" s="4">
+        <v>10</v>
+      </c>
+      <c r="S9" s="4">
+        <v>15</v>
+      </c>
+      <c r="T9" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1962,8 +3424,20 @@
       <c r="M10" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q10" s="2">
+        <v>5</v>
+      </c>
+      <c r="R10" s="4">
+        <v>10</v>
+      </c>
+      <c r="S10" s="4">
+        <v>15</v>
+      </c>
+      <c r="T10" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2003,8 +3477,20 @@
       <c r="M11" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q11" s="2">
+        <v>6</v>
+      </c>
+      <c r="R11" s="4">
+        <v>10</v>
+      </c>
+      <c r="S11" s="4">
+        <v>15</v>
+      </c>
+      <c r="T11" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2044,8 +3530,20 @@
       <c r="M12" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q12" s="2">
+        <v>7</v>
+      </c>
+      <c r="R12" s="4">
+        <v>10</v>
+      </c>
+      <c r="S12" s="4">
+        <v>15</v>
+      </c>
+      <c r="T12" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2085,8 +3583,20 @@
       <c r="M13" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q13" s="2">
+        <v>8</v>
+      </c>
+      <c r="R13" s="4">
+        <v>10</v>
+      </c>
+      <c r="S13" s="4">
+        <v>15</v>
+      </c>
+      <c r="T13" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2126,8 +3636,20 @@
       <c r="M14" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q14" s="2">
+        <v>9</v>
+      </c>
+      <c r="R14" s="4">
+        <v>6</v>
+      </c>
+      <c r="S14" s="4">
+        <v>15</v>
+      </c>
+      <c r="T14" s="4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2167,8 +3689,20 @@
       <c r="M15" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q15" s="2">
+        <v>10</v>
+      </c>
+      <c r="R15" s="4">
+        <v>2</v>
+      </c>
+      <c r="S15" s="4">
+        <v>15</v>
+      </c>
+      <c r="T15" s="4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2208,8 +3742,20 @@
       <c r="M16" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q16" s="2">
+        <v>11</v>
+      </c>
+      <c r="R16" s="4">
+        <v>2</v>
+      </c>
+      <c r="S16" s="4">
+        <v>15</v>
+      </c>
+      <c r="T16" s="4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2249,8 +3795,20 @@
       <c r="M17" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q17" s="2">
+        <v>12</v>
+      </c>
+      <c r="R17" s="4">
+        <v>0</v>
+      </c>
+      <c r="S17" s="4">
+        <v>15</v>
+      </c>
+      <c r="T17" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2</v>
       </c>
@@ -2290,8 +3848,20 @@
       <c r="M18" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R18" s="4">
+        <v>100</v>
+      </c>
+      <c r="S18" s="4">
+        <v>195</v>
+      </c>
+      <c r="T18" s="4">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -2332,7 +3902,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2</v>
       </c>
@@ -2373,7 +3943,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
@@ -2414,7 +3984,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2</v>
       </c>
@@ -2455,7 +4025,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2</v>
       </c>
@@ -2496,7 +4066,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2</v>
       </c>
@@ -2537,7 +4107,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
@@ -2578,7 +4148,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3</v>
       </c>
@@ -2619,7 +4189,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>3</v>
       </c>
@@ -2660,7 +4230,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3</v>
       </c>
@@ -2701,7 +4271,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>3</v>
       </c>
@@ -2742,7 +4312,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>3</v>
       </c>
@@ -2783,7 +4353,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>3</v>
       </c>
@@ -2824,7 +4394,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>3</v>
       </c>
@@ -4087,8 +5657,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>